<commit_message>
fix namefichier + view modules
</commit_message>
<xml_diff>
--- a/projet/wwwroot/FichierAddDBEnseignants/addliste.xlsx
+++ b/projet/wwwroot/FichierAddDBEnseignants/addliste.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>nom</t>
   </si>
@@ -34,16 +34,10 @@
     <t>telephone</t>
   </si>
   <si>
-    <t>photo</t>
-  </si>
-  <si>
     <t>manal</t>
   </si>
   <si>
     <t>ait dik</t>
-  </si>
-  <si>
-    <t>imgapng</t>
   </si>
   <si>
     <t>jiji</t>
@@ -138,16 +132,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G8" totalsRowShown="0">
-  <autoFilter ref="A1:G8"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F8" totalsRowShown="0">
+  <autoFilter ref="A1:F8"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="nom"/>
     <tableColumn id="2" name="prenom"/>
     <tableColumn id="3" name="username"/>
     <tableColumn id="4" name="mdp"/>
     <tableColumn id="5" name="email"/>
     <tableColumn id="6" name="telephone"/>
-    <tableColumn id="7" name="photo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -440,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G8"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,7 +448,7 @@
     <col min="8" max="10" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,169 +467,145 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2">
         <v>67878787</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
       <c r="D3">
         <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
       <c r="D4">
         <v>123</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4">
         <v>67878787</v>
       </c>
-      <c r="G4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>67878787</v>
       </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
       </c>
       <c r="D6">
         <v>123</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6">
         <v>67878888787</v>
       </c>
-      <c r="G6" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
       </c>
       <c r="D7">
         <v>123</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7">
         <v>67878787</v>
       </c>
-      <c r="G7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
       </c>
       <c r="D8">
         <v>123</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8">
         <v>67878787</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>